<commit_message>
feat: logo + login
</commit_message>
<xml_diff>
--- a/public/static/元数据模板.xlsx
+++ b/public/static/元数据模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="16000"/>
+    <workbookView windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12">
   <si>
     <t>名称</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>标签</t>
-  </si>
-  <si>
-    <t>URL</t>
   </si>
   <si>
     <t>备注</t>
@@ -52,9 +49,6 @@
     <t>会员1.1.2(选填,多个用","隔开)</t>
   </si>
   <si>
-    <t>http://www.baidu.com(选填)</t>
-  </si>
-  <si>
     <t>会员点击(选填)</t>
   </si>
 </sst>
@@ -63,10 +57,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -77,6 +71,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -86,14 +94,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -108,40 +148,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,12 +164,35 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -168,30 +200,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -199,25 +209,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -236,181 +230,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,17 +457,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,6 +499,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -507,192 +536,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -700,9 +694,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="41" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1024,13 +1015,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="22.7678571428571" customWidth="1"/>
     <col min="2" max="2" width="27.375" customWidth="1"/>
@@ -1038,10 +1029,9 @@
     <col min="4" max="4" width="13.5357142857143" customWidth="1"/>
     <col min="5" max="5" width="30.9553571428571" customWidth="1"/>
     <col min="6" max="6" width="28.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="28.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1060,118 +1050,100 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="http://www.baidu.com(选填)"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>